<commit_message>
agregada logica de importar excel de ventas y validaciones de formato
</commit_message>
<xml_diff>
--- a/Espressoft-master/documentos_excel/ventas/ventas-2021.xlsx
+++ b/Espressoft-master/documentos_excel/ventas/ventas-2021.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNISON\2023-1\Practicas de desarrollo de sistemas\Espressoft\Espressoft-master\documentos_excel\ventas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP 6300\Documents\6semestre\pds1\Proyecto\Espressoft\Espressoft-master\documentos_excel\ventas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB78451E-890A-4907-96D5-875FC5BACB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="5715" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="5715" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -3112,7 +3111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3237,23 +3236,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3289,23 +3271,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3481,14 +3446,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5905"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A5895" workbookViewId="0">
+      <selection activeCell="F5905" sqref="F5905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>